<commit_message>
he creado escrito en las casillas y he creado nuevas hojas en el mismo archivo
</commit_message>
<xml_diff>
--- a/excel_deimer.xlsx
+++ b/excel_deimer.xlsx
@@ -7,7 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -423,4 +426,103 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Canciones</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Género</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Año</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>¿Es famosa la canción?</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Vamos a cantar</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>¿Qué canción?</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pues yo no sé, dime tú</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Ok!... entonces cantaremos los pollitos</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
crear una hoja de calculo
</commit_message>
<xml_diff>
--- a/excel_deimer.xlsx
+++ b/excel_deimer.xlsx
@@ -7,10 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="bailes" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="discotecas" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="canciones" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="canciones" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,24 +414,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -491,25 +471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>